<commit_message>
actualizacion 11 agosto 12
</commit_message>
<xml_diff>
--- a/Resultado/estado_gestion_Paquete_1_Medellin.xlsx
+++ b/Resultado/estado_gestion_Paquete_1_Medellin.xlsx
@@ -2257,11 +2257,11 @@
         <v>32920</v>
       </c>
       <c r="B114" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D114" s="2" t="n">
@@ -2401,11 +2401,11 @@
         <v>34847</v>
       </c>
       <c r="B123" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Por Reprogramar</t>
         </is>
       </c>
       <c r="D123" s="2" t="n">
@@ -4961,11 +4961,11 @@
         <v>61171</v>
       </c>
       <c r="B283" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Por Reprogramar</t>
         </is>
       </c>
       <c r="D283" s="2" t="n">
@@ -5025,11 +5025,11 @@
         <v>61259</v>
       </c>
       <c r="B287" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D287" s="2" t="n">
@@ -6785,11 +6785,11 @@
         <v>74439</v>
       </c>
       <c r="B397" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D397" s="2" t="n">
@@ -8327,7 +8327,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8354,7 +8354,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3">
@@ -8374,7 +8374,17 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Por Reprogramar</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
act 11 oct 13 horas
</commit_message>
<xml_diff>
--- a/Resultado/estado_gestion_Paquete_1_Medellin.xlsx
+++ b/Resultado/estado_gestion_Paquete_1_Medellin.xlsx
@@ -833,11 +833,11 @@
         <v>14902</v>
       </c>
       <c r="B25" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
@@ -1425,11 +1425,11 @@
         <v>23658</v>
       </c>
       <c r="B62" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
@@ -2321,11 +2321,11 @@
         <v>34010</v>
       </c>
       <c r="B118" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D118" s="2" t="n">
@@ -2625,11 +2625,11 @@
         <v>36659</v>
       </c>
       <c r="B137" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D137" s="2" t="n">
@@ -4417,11 +4417,11 @@
         <v>54552</v>
       </c>
       <c r="B249" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>En Bodega</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="D249" s="2" t="n">
@@ -8354,7 +8354,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3">
@@ -8374,7 +8374,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">

</xml_diff>